<commit_message>
Updates all 16S materials to updated ref_db DADA2 run; Updates all comparison and abundance tables (and includes code to remove Mammalia and Bactera classifications
</commit_message>
<xml_diff>
--- a/Deliverables/16S/WADE003-arcticpred_dada2_QAQC_16SP1+2.xlsx
+++ b/Deliverables/16S/WADE003-arcticpred_dada2_QAQC_16SP1+2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5bd2331949789710/文档/WADE LAB/Arctic-predator-diet-microbiome/Deliverables/16S/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MBall\OneDrive\Documents\UW-DOCS\WADE lab\Arctic-predator-diet-microbiome\Deliverables\16S\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="11_80217FC58F79A8D366075C52F37BD2721AC5D141" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{673FA50B-5AEB-4EED-8639-76FF66009604}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62531B21-90D8-42B2-8A74-4685DCE05162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1903" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1923" uniqueCount="220">
   <si>
     <t>rownames</t>
   </si>
@@ -679,6 +679,9 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>&gt;99% Eleginus gracilis AND Microgadus proximus</t>
   </si>
 </sst>
 </file>
@@ -1037,21 +1040,21 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.73046875" customWidth="1"/>
+    <col min="2" max="2" width="14.265625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.73046875" customWidth="1"/>
+    <col min="5" max="5" width="19.86328125" customWidth="1"/>
+    <col min="6" max="6" width="16.1328125" customWidth="1"/>
+    <col min="7" max="7" width="16.59765625" customWidth="1"/>
+    <col min="8" max="8" width="22.265625" customWidth="1"/>
+    <col min="9" max="9" width="20.59765625" customWidth="1"/>
+    <col min="10" max="10" width="24.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1083,7 +1086,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1115,7 +1118,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1147,7 +1150,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1179,7 +1182,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1211,7 +1214,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1243,7 +1246,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1275,7 +1278,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1307,7 +1310,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1318,7 +1321,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1350,7 +1353,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -1382,7 +1385,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1414,7 +1417,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1446,7 +1449,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1466,7 +1469,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -1498,7 +1501,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -1530,7 +1533,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -1562,7 +1565,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -1594,7 +1597,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -1626,7 +1629,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -1652,12 +1655,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -1689,7 +1692,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -1721,7 +1724,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -1735,7 +1738,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -1761,7 +1764,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>73</v>
       </c>
@@ -1793,7 +1796,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>74</v>
       </c>
@@ -1819,7 +1822,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>75</v>
       </c>
@@ -1845,7 +1848,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>76</v>
       </c>
@@ -1877,7 +1880,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>77</v>
       </c>
@@ -1903,7 +1906,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>78</v>
       </c>
@@ -1929,7 +1932,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>79</v>
       </c>
@@ -1949,7 +1952,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>82</v>
       </c>
@@ -1975,7 +1978,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>83</v>
       </c>
@@ -2001,7 +2004,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>84</v>
       </c>
@@ -2027,7 +2030,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>85</v>
       </c>
@@ -2053,7 +2056,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -2073,7 +2076,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -2093,7 +2096,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>91</v>
       </c>
@@ -2107,7 +2110,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>92</v>
       </c>
@@ -2127,7 +2130,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>95</v>
       </c>
@@ -2159,7 +2162,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>100</v>
       </c>
@@ -2191,7 +2194,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>101</v>
       </c>
@@ -2217,7 +2220,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>102</v>
       </c>
@@ -2237,7 +2240,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>104</v>
       </c>
@@ -2263,7 +2266,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>105</v>
       </c>
@@ -2289,7 +2292,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>106</v>
       </c>
@@ -2315,7 +2318,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>107</v>
       </c>
@@ -2341,7 +2344,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>108</v>
       </c>
@@ -2367,7 +2370,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>109</v>
       </c>
@@ -2381,7 +2384,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>111</v>
       </c>
@@ -2407,7 +2410,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>112</v>
       </c>
@@ -2433,7 +2436,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>113</v>
       </c>
@@ -2465,7 +2468,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>114</v>
       </c>
@@ -2497,7 +2500,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>118</v>
       </c>
@@ -2529,7 +2532,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>119</v>
       </c>
@@ -2555,7 +2558,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>120</v>
       </c>
@@ -2587,7 +2590,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>121</v>
       </c>
@@ -2619,7 +2622,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>126</v>
       </c>
@@ -2648,7 +2651,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>127</v>
       </c>
@@ -2680,7 +2683,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>130</v>
       </c>
@@ -2712,7 +2715,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>131</v>
       </c>
@@ -2732,7 +2735,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>134</v>
       </c>
@@ -2758,7 +2761,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>135</v>
       </c>
@@ -2772,7 +2775,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>137</v>
       </c>
@@ -2792,7 +2795,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>140</v>
       </c>
@@ -2824,7 +2827,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>143</v>
       </c>
@@ -2844,7 +2847,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>146</v>
       </c>
@@ -2876,7 +2879,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>152</v>
       </c>
@@ -2902,7 +2905,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>155</v>
       </c>
@@ -2934,7 +2937,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>156</v>
       </c>
@@ -2966,7 +2969,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>159</v>
       </c>
@@ -2998,7 +3001,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>163</v>
       </c>
@@ -3030,7 +3033,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>168</v>
       </c>
@@ -3062,7 +3065,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>173</v>
       </c>
@@ -3088,7 +3091,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>174</v>
       </c>
@@ -3120,7 +3123,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>175</v>
       </c>
@@ -3152,7 +3155,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>177</v>
       </c>
@@ -3184,7 +3187,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>178</v>
       </c>
@@ -3213,7 +3216,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>180</v>
       </c>
@@ -3245,7 +3248,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>183</v>
       </c>
@@ -3277,7 +3280,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>184</v>
       </c>
@@ -3309,7 +3312,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>185</v>
       </c>
@@ -3341,7 +3344,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>186</v>
       </c>
@@ -3361,7 +3364,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>187</v>
       </c>
@@ -3393,7 +3396,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>188</v>
       </c>
@@ -3425,7 +3428,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>189</v>
       </c>
@@ -3445,7 +3448,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>190</v>
       </c>
@@ -3471,7 +3474,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>191</v>
       </c>
@@ -3503,7 +3506,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>192</v>
       </c>
@@ -3535,7 +3538,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>193</v>
       </c>
@@ -3561,7 +3564,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>194</v>
       </c>
@@ -3593,7 +3596,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>195</v>
       </c>
@@ -3625,7 +3628,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>196</v>
       </c>
@@ -3645,7 +3648,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>197</v>
       </c>
@@ -3677,12 +3680,12 @@
         <v>176</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>199</v>
       </c>
@@ -3714,7 +3717,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>200</v>
       </c>
@@ -3746,7 +3749,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>201</v>
       </c>
@@ -3778,7 +3781,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>202</v>
       </c>
@@ -3804,7 +3807,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>203</v>
       </c>
@@ -3836,7 +3839,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>204</v>
       </c>
@@ -3868,7 +3871,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>205</v>
       </c>
@@ -3900,7 +3903,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>213</v>
       </c>
@@ -3932,7 +3935,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>216</v>
       </c>
@@ -3964,7 +3967,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>217</v>
       </c>
@@ -4009,21 +4012,21 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.73046875" customWidth="1"/>
+    <col min="2" max="2" width="14.265625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.73046875" customWidth="1"/>
+    <col min="5" max="5" width="19.86328125" customWidth="1"/>
+    <col min="6" max="6" width="16.1328125" customWidth="1"/>
+    <col min="7" max="7" width="16.59765625" customWidth="1"/>
+    <col min="8" max="8" width="22.265625" customWidth="1"/>
+    <col min="9" max="9" width="20.59765625" customWidth="1"/>
+    <col min="10" max="10" width="24.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4055,7 +4058,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -4087,7 +4090,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -4119,7 +4122,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -4151,7 +4154,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -4183,7 +4186,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -4215,7 +4218,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -4247,7 +4250,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -4279,7 +4282,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -4290,7 +4293,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -4322,7 +4325,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -4354,7 +4357,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -4386,7 +4389,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -4418,7 +4421,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -4438,7 +4441,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -4470,7 +4473,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -4502,7 +4505,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -4534,7 +4537,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -4566,7 +4569,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -4598,7 +4601,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -4624,12 +4627,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -4661,7 +4664,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -4693,7 +4696,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -4707,7 +4710,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -4733,7 +4736,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>73</v>
       </c>
@@ -4765,7 +4768,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>74</v>
       </c>
@@ -4791,7 +4794,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>75</v>
       </c>
@@ -4817,7 +4820,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>76</v>
       </c>
@@ -4849,7 +4852,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>77</v>
       </c>
@@ -4875,7 +4878,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>78</v>
       </c>
@@ -4901,7 +4904,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>79</v>
       </c>
@@ -4921,7 +4924,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>82</v>
       </c>
@@ -4947,7 +4950,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>83</v>
       </c>
@@ -4973,7 +4976,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>84</v>
       </c>
@@ -4999,7 +5002,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>85</v>
       </c>
@@ -5025,7 +5028,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -5045,7 +5048,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -5065,7 +5068,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>91</v>
       </c>
@@ -5079,7 +5082,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>92</v>
       </c>
@@ -5099,7 +5102,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>95</v>
       </c>
@@ -5131,7 +5134,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>100</v>
       </c>
@@ -5163,7 +5166,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>101</v>
       </c>
@@ -5189,7 +5192,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>102</v>
       </c>
@@ -5209,7 +5212,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>104</v>
       </c>
@@ -5235,7 +5238,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>105</v>
       </c>
@@ -5261,7 +5264,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>106</v>
       </c>
@@ -5287,7 +5290,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>107</v>
       </c>
@@ -5313,7 +5316,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>108</v>
       </c>
@@ -5339,7 +5342,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>109</v>
       </c>
@@ -5353,7 +5356,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>111</v>
       </c>
@@ -5379,7 +5382,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>112</v>
       </c>
@@ -5405,7 +5408,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>113</v>
       </c>
@@ -5437,7 +5440,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>114</v>
       </c>
@@ -5469,7 +5472,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>118</v>
       </c>
@@ -5501,7 +5504,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>119</v>
       </c>
@@ -5527,7 +5530,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>120</v>
       </c>
@@ -5559,7 +5562,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>121</v>
       </c>
@@ -5591,7 +5594,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>126</v>
       </c>
@@ -5620,7 +5623,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>127</v>
       </c>
@@ -5652,7 +5655,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>130</v>
       </c>
@@ -5684,7 +5687,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>131</v>
       </c>
@@ -5704,7 +5707,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>134</v>
       </c>
@@ -5730,7 +5733,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>135</v>
       </c>
@@ -5744,7 +5747,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>137</v>
       </c>
@@ -5764,7 +5767,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>140</v>
       </c>
@@ -5796,7 +5799,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>143</v>
       </c>
@@ -5816,7 +5819,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>152</v>
       </c>
@@ -5842,7 +5845,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>155</v>
       </c>
@@ -5874,7 +5877,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>159</v>
       </c>
@@ -5906,7 +5909,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>168</v>
       </c>
@@ -5938,7 +5941,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>173</v>
       </c>
@@ -5964,7 +5967,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>174</v>
       </c>
@@ -5996,7 +5999,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>175</v>
       </c>
@@ -6028,7 +6031,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>177</v>
       </c>
@@ -6060,7 +6063,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>178</v>
       </c>
@@ -6089,7 +6092,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>180</v>
       </c>
@@ -6121,7 +6124,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>183</v>
       </c>
@@ -6153,7 +6156,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>185</v>
       </c>
@@ -6185,7 +6188,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>186</v>
       </c>
@@ -6205,7 +6208,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>187</v>
       </c>
@@ -6237,7 +6240,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>188</v>
       </c>
@@ -6269,7 +6272,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>189</v>
       </c>
@@ -6289,7 +6292,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>194</v>
       </c>
@@ -6321,7 +6324,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>196</v>
       </c>
@@ -6341,7 +6344,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>197</v>
       </c>
@@ -6373,12 +6376,12 @@
         <v>176</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>199</v>
       </c>
@@ -6410,7 +6413,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>200</v>
       </c>
@@ -6442,7 +6445,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>201</v>
       </c>
@@ -6474,7 +6477,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>213</v>
       </c>
@@ -6506,7 +6509,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>216</v>
       </c>
@@ -6538,7 +6541,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>217</v>
       </c>
@@ -6580,22 +6583,23 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.86328125" customWidth="1"/>
+    <col min="3" max="3" width="11.3984375" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6630,7 +6634,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -6655,13 +6659,16 @@
       <c r="H2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -6686,8 +6693,11 @@
       <c r="H4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>74</v>
       </c>
@@ -6712,8 +6722,11 @@
       <c r="H5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -6738,8 +6751,11 @@
       <c r="H6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>77</v>
       </c>
@@ -6764,8 +6780,11 @@
       <c r="H7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>78</v>
       </c>
@@ -6790,8 +6809,11 @@
       <c r="H8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>82</v>
       </c>
@@ -6816,8 +6838,11 @@
       <c r="H9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -6842,8 +6867,11 @@
       <c r="H10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>84</v>
       </c>
@@ -6868,8 +6896,11 @@
       <c r="H11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>85</v>
       </c>
@@ -6894,8 +6925,11 @@
       <c r="H12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K12" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>91</v>
       </c>
@@ -6909,7 +6943,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>101</v>
       </c>
@@ -6934,8 +6968,11 @@
       <c r="H14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>104</v>
       </c>
@@ -6960,8 +6997,11 @@
       <c r="H15" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>105</v>
       </c>
@@ -6986,8 +7026,11 @@
       <c r="H16" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>106</v>
       </c>
@@ -7012,8 +7055,11 @@
       <c r="H17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>107</v>
       </c>
@@ -7038,8 +7084,11 @@
       <c r="H18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>108</v>
       </c>
@@ -7064,8 +7113,11 @@
       <c r="H19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>111</v>
       </c>
@@ -7090,8 +7142,11 @@
       <c r="H20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K20" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>112</v>
       </c>
@@ -7116,8 +7171,11 @@
       <c r="H21" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K21" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>119</v>
       </c>
@@ -7142,8 +7200,11 @@
       <c r="H22" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K22" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>134</v>
       </c>
@@ -7168,8 +7229,11 @@
       <c r="H23" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>152</v>
       </c>
@@ -7195,7 +7259,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>173</v>
       </c>
@@ -7221,7 +7285,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>189</v>
       </c>
@@ -7241,7 +7305,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>196</v>
       </c>
@@ -7261,7 +7325,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>198</v>
       </c>

</xml_diff>

<commit_message>
Fixes select masking (dplyr::select)
</commit_message>
<xml_diff>
--- a/Deliverables/16S/WADE003-arcticpred_dada2_QAQC_16SP1+2.xlsx
+++ b/Deliverables/16S/WADE003-arcticpred_dada2_QAQC_16SP1+2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MBall\OneDrive\Documents\UW-DOCS\WADE lab\Arctic-predator-diet-microbiome\Deliverables\16S\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MBall\OneDrive\Documents\UW-DOCS\WADE lab\Arctic-predator-diet-microbiome\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62531B21-90D8-42B2-8A74-4685DCE05162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258D4E77-B103-4DBC-95BE-D3089DBEE166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1923" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1927" uniqueCount="223">
   <si>
     <t>rownames</t>
   </si>
@@ -354,6 +354,9 @@
     <t>ATAACGAGGGCTTAACTGTCTCCTCTTTCAAGTCAATGAAATTGATCTCCCCGTGCAGAAGCGGGGATAAAAACATAAGACGAGAAGACCCTATGGAGCTTTAGACACCAAGGCAGCCCACGTTAAAGACCCTCAATAAAGGACTAAACCAAGTGAGCCCTGCCCTAATGTCTTTGGTTGGGGCGACCGCGGGGAATTAAAGAACCCCCACGTGGAACGGGAATACTCTTCCTACAACTAAGAGCTACAGCTCTAATAAACAGAACTTCTGACCAGCAAGATCCGGCAGTGCCG</t>
   </si>
   <si>
+    <t>Cottidae</t>
+  </si>
+  <si>
     <t>Myoxocephalus quadricornis</t>
   </si>
   <si>
@@ -447,9 +450,6 @@
     <t>ATAACGAGGGCTTAACTGTCTCCTCTTTCAAGTTAATGAAATTGATCTCCCCGTGCAGAAGCGGGGATAAAAACATAAGACGAGAAGACCCTATGGAGCTTTAGACACTAAGACAGCCCACGTTAAGCACCCTGAATAAAGGACTAAACCAAGTGGGCCCTGCCCTAATGTCTTTGGTTGGGGCGACCGCGGGGAATTAAAGAACCCCCACGTGGAGTGGGAATACTTTTCCTACAACTAAGAGCTACAGCTCTCATAAACAGAATTTCTGACCAACAAGATCCGGCAGTGCCG</t>
   </si>
   <si>
-    <t>Cottidae</t>
-  </si>
-  <si>
     <t>Gymnocanthus pistilliger</t>
   </si>
   <si>
@@ -682,6 +682,15 @@
   </si>
   <si>
     <t>&gt;99% Eleginus gracilis AND Microgadus proximus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;99% Coregonus spp. AND Stenodus leucichthys </t>
+  </si>
+  <si>
+    <t>100% Leptoclinus maculatus AND Lumpenus fabricii</t>
+  </si>
+  <si>
+    <t>Nothing &gt; 98%</t>
   </si>
 </sst>
 </file>
@@ -1042,16 +1051,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.73046875" customWidth="1"/>
-    <col min="2" max="2" width="14.265625" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="16.73046875" customWidth="1"/>
-    <col min="5" max="5" width="19.86328125" customWidth="1"/>
-    <col min="6" max="6" width="16.1328125" customWidth="1"/>
-    <col min="7" max="7" width="16.59765625" customWidth="1"/>
-    <col min="8" max="8" width="22.265625" customWidth="1"/>
-    <col min="9" max="9" width="20.59765625" customWidth="1"/>
-    <col min="10" max="10" width="24.73046875" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.19921875" customWidth="1"/>
+    <col min="3" max="3" width="14.796875" customWidth="1"/>
+    <col min="4" max="4" width="15.86328125" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.06640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
@@ -2377,16 +2386,34 @@
       <c r="B50" t="s">
         <v>11</v>
       </c>
+      <c r="C50" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50" t="s">
+        <v>48</v>
+      </c>
+      <c r="F50" t="s">
+        <v>110</v>
+      </c>
+      <c r="G50" t="s">
+        <v>70</v>
+      </c>
+      <c r="H50" t="s">
+        <v>111</v>
+      </c>
       <c r="I50" t="s">
         <v>70</v>
       </c>
       <c r="J50" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B51" t="s">
         <v>11</v>
@@ -2412,7 +2439,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B52" t="s">
         <v>11</v>
@@ -2438,7 +2465,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B53" t="s">
         <v>11</v>
@@ -2470,7 +2497,7 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B54" t="s">
         <v>11</v>
@@ -2485,24 +2512,24 @@
         <v>48</v>
       </c>
       <c r="F54" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G54" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H54" t="s">
+        <v>118</v>
+      </c>
+      <c r="I54" t="s">
         <v>117</v>
       </c>
-      <c r="I54" t="s">
-        <v>116</v>
-      </c>
       <c r="J54" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B55" t="s">
         <v>11</v>
@@ -2534,7 +2561,7 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B56" t="s">
         <v>11</v>
@@ -2560,7 +2587,7 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B57" t="s">
         <v>11</v>
@@ -2592,7 +2619,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B58" t="s">
         <v>11</v>
@@ -2604,27 +2631,27 @@
         <v>13</v>
       </c>
       <c r="E58" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F58" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G58" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H58" t="s">
+        <v>126</v>
+      </c>
+      <c r="I58" t="s">
         <v>125</v>
       </c>
-      <c r="I58" t="s">
-        <v>124</v>
-      </c>
       <c r="J58" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B59" t="s">
         <v>11</v>
@@ -2653,7 +2680,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B60" t="s">
         <v>11</v>
@@ -2668,24 +2695,24 @@
         <v>48</v>
       </c>
       <c r="F60" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G60" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H60" t="s">
+        <v>130</v>
+      </c>
+      <c r="I60" t="s">
         <v>129</v>
       </c>
-      <c r="I60" t="s">
-        <v>128</v>
-      </c>
       <c r="J60" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B61" t="s">
         <v>11</v>
@@ -2717,7 +2744,7 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B62" t="s">
         <v>11</v>
@@ -2729,15 +2756,15 @@
         <v>13</v>
       </c>
       <c r="I62" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J62" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B63" t="s">
         <v>11</v>
@@ -2763,7 +2790,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B64" t="s">
         <v>11</v>
@@ -2772,12 +2799,12 @@
         <v>70</v>
       </c>
       <c r="J64" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B65" t="s">
         <v>11</v>
@@ -2789,15 +2816,15 @@
         <v>13</v>
       </c>
       <c r="I65" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J65" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B66" t="s">
         <v>11</v>
@@ -2812,16 +2839,16 @@
         <v>48</v>
       </c>
       <c r="F66" t="s">
-        <v>141</v>
+        <v>110</v>
       </c>
       <c r="G66" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H66" t="s">
         <v>142</v>
       </c>
       <c r="I66" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J66" t="s">
         <v>142</v>
@@ -2840,6 +2867,18 @@
       <c r="D67" t="s">
         <v>13</v>
       </c>
+      <c r="E67" t="s">
+        <v>14</v>
+      </c>
+      <c r="F67" t="s">
+        <v>15</v>
+      </c>
+      <c r="G67" t="s">
+        <v>144</v>
+      </c>
+      <c r="H67" t="s">
+        <v>145</v>
+      </c>
       <c r="I67" t="s">
         <v>144</v>
       </c>
@@ -2892,16 +2931,10 @@
       <c r="D69" t="s">
         <v>13</v>
       </c>
-      <c r="E69" t="s">
-        <v>122</v>
-      </c>
-      <c r="F69" t="s">
-        <v>141</v>
-      </c>
-      <c r="G69" t="s">
+      <c r="I69" t="s">
         <v>153</v>
       </c>
-      <c r="H69" t="s">
+      <c r="J69" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2919,10 +2952,10 @@
         <v>13</v>
       </c>
       <c r="E70" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F70" t="s">
-        <v>141</v>
+        <v>110</v>
       </c>
       <c r="G70" t="s">
         <v>153</v>
@@ -3140,7 +3173,7 @@
         <v>48</v>
       </c>
       <c r="F77" t="s">
-        <v>141</v>
+        <v>110</v>
       </c>
       <c r="G77" t="s">
         <v>70</v>
@@ -3262,22 +3295,22 @@
         <v>13</v>
       </c>
       <c r="E81" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F81" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G81" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H81" t="s">
+        <v>126</v>
+      </c>
+      <c r="I81" t="s">
         <v>125</v>
       </c>
-      <c r="I81" t="s">
-        <v>124</v>
-      </c>
       <c r="J81" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.45">
@@ -3358,10 +3391,10 @@
         <v>13</v>
       </c>
       <c r="I84" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J84" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.45">
@@ -3445,7 +3478,7 @@
         <v>48</v>
       </c>
       <c r="F87" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.45">
@@ -3665,7 +3698,7 @@
         <v>48</v>
       </c>
       <c r="F95" t="s">
-        <v>141</v>
+        <v>110</v>
       </c>
       <c r="G95" t="s">
         <v>70</v>
@@ -3920,7 +3953,7 @@
         <v>48</v>
       </c>
       <c r="F104" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G104" t="s">
         <v>214</v>
@@ -4005,25 +4038,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4D12DB3-075A-4201-BDC8-ADC221A3399A}">
-  <dimension ref="A1:J93"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCF5EE55-48E8-422E-B365-122DC9DDF43F}">
+  <dimension ref="A1:J92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.73046875" customWidth="1"/>
-    <col min="2" max="2" width="14.265625" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="16.73046875" customWidth="1"/>
-    <col min="5" max="5" width="19.86328125" customWidth="1"/>
-    <col min="6" max="6" width="16.1328125" customWidth="1"/>
-    <col min="7" max="7" width="16.59765625" customWidth="1"/>
-    <col min="8" max="8" width="22.265625" customWidth="1"/>
-    <col min="9" max="9" width="20.59765625" customWidth="1"/>
-    <col min="10" max="10" width="24.73046875" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.19921875" customWidth="1"/>
+    <col min="3" max="3" width="14.796875" customWidth="1"/>
+    <col min="4" max="4" width="15.86328125" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.06640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
@@ -5349,16 +5382,34 @@
       <c r="B50" t="s">
         <v>11</v>
       </c>
+      <c r="C50" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50" t="s">
+        <v>48</v>
+      </c>
+      <c r="F50" t="s">
+        <v>110</v>
+      </c>
+      <c r="G50" t="s">
+        <v>70</v>
+      </c>
+      <c r="H50" t="s">
+        <v>111</v>
+      </c>
       <c r="I50" t="s">
         <v>70</v>
       </c>
       <c r="J50" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B51" t="s">
         <v>11</v>
@@ -5384,7 +5435,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B52" t="s">
         <v>11</v>
@@ -5410,7 +5461,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B53" t="s">
         <v>11</v>
@@ -5442,7 +5493,7 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B54" t="s">
         <v>11</v>
@@ -5457,24 +5508,24 @@
         <v>48</v>
       </c>
       <c r="F54" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G54" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H54" t="s">
+        <v>118</v>
+      </c>
+      <c r="I54" t="s">
         <v>117</v>
       </c>
-      <c r="I54" t="s">
-        <v>116</v>
-      </c>
       <c r="J54" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B55" t="s">
         <v>11</v>
@@ -5506,7 +5557,7 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B56" t="s">
         <v>11</v>
@@ -5532,7 +5583,7 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B57" t="s">
         <v>11</v>
@@ -5564,7 +5615,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B58" t="s">
         <v>11</v>
@@ -5576,27 +5627,27 @@
         <v>13</v>
       </c>
       <c r="E58" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F58" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G58" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H58" t="s">
+        <v>126</v>
+      </c>
+      <c r="I58" t="s">
         <v>125</v>
       </c>
-      <c r="I58" t="s">
-        <v>124</v>
-      </c>
       <c r="J58" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B59" t="s">
         <v>11</v>
@@ -5625,7 +5676,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B60" t="s">
         <v>11</v>
@@ -5640,24 +5691,24 @@
         <v>48</v>
       </c>
       <c r="F60" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G60" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H60" t="s">
+        <v>130</v>
+      </c>
+      <c r="I60" t="s">
         <v>129</v>
       </c>
-      <c r="I60" t="s">
-        <v>128</v>
-      </c>
       <c r="J60" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B61" t="s">
         <v>11</v>
@@ -5689,7 +5740,7 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B62" t="s">
         <v>11</v>
@@ -5701,15 +5752,15 @@
         <v>13</v>
       </c>
       <c r="I62" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J62" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B63" t="s">
         <v>11</v>
@@ -5735,7 +5786,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B64" t="s">
         <v>11</v>
@@ -5744,12 +5795,12 @@
         <v>70</v>
       </c>
       <c r="J64" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B65" t="s">
         <v>11</v>
@@ -5761,15 +5812,15 @@
         <v>13</v>
       </c>
       <c r="I65" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J65" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B66" t="s">
         <v>11</v>
@@ -5784,16 +5835,16 @@
         <v>48</v>
       </c>
       <c r="F66" t="s">
-        <v>141</v>
+        <v>110</v>
       </c>
       <c r="G66" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H66" t="s">
         <v>142</v>
       </c>
       <c r="I66" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J66" t="s">
         <v>142</v>
@@ -5812,6 +5863,18 @@
       <c r="D67" t="s">
         <v>13</v>
       </c>
+      <c r="E67" t="s">
+        <v>14</v>
+      </c>
+      <c r="F67" t="s">
+        <v>15</v>
+      </c>
+      <c r="G67" t="s">
+        <v>144</v>
+      </c>
+      <c r="H67" t="s">
+        <v>145</v>
+      </c>
       <c r="I67" t="s">
         <v>144</v>
       </c>
@@ -5832,16 +5895,10 @@
       <c r="D68" t="s">
         <v>13</v>
       </c>
-      <c r="E68" t="s">
-        <v>122</v>
-      </c>
-      <c r="F68" t="s">
-        <v>141</v>
-      </c>
-      <c r="G68" t="s">
+      <c r="I68" t="s">
         <v>153</v>
       </c>
-      <c r="H68" t="s">
+      <c r="J68" t="s">
         <v>154</v>
       </c>
     </row>
@@ -5859,10 +5916,10 @@
         <v>13</v>
       </c>
       <c r="E69" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F69" t="s">
-        <v>141</v>
+        <v>110</v>
       </c>
       <c r="G69" t="s">
         <v>153</v>
@@ -6016,7 +6073,7 @@
         <v>48</v>
       </c>
       <c r="F74" t="s">
-        <v>141</v>
+        <v>110</v>
       </c>
       <c r="G74" t="s">
         <v>70</v>
@@ -6138,22 +6195,22 @@
         <v>13</v>
       </c>
       <c r="E78" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F78" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G78" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H78" t="s">
+        <v>126</v>
+      </c>
+      <c r="I78" t="s">
         <v>125</v>
       </c>
-      <c r="I78" t="s">
-        <v>124</v>
-      </c>
       <c r="J78" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.45">
@@ -6202,15 +6259,15 @@
         <v>13</v>
       </c>
       <c r="I80" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J80" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B81" t="s">
         <v>11</v>
@@ -6219,30 +6276,30 @@
         <v>12</v>
       </c>
       <c r="D81" t="s">
-        <v>147</v>
+        <v>13</v>
       </c>
       <c r="E81" t="s">
-        <v>148</v>
+        <v>27</v>
       </c>
       <c r="F81" t="s">
-        <v>149</v>
+        <v>28</v>
       </c>
       <c r="G81" t="s">
-        <v>150</v>
+        <v>55</v>
       </c>
       <c r="H81" t="s">
-        <v>151</v>
+        <v>56</v>
       </c>
       <c r="I81" t="s">
-        <v>150</v>
+        <v>55</v>
       </c>
       <c r="J81" t="s">
-        <v>151</v>
+        <v>56</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B82" t="s">
         <v>11</v>
@@ -6254,27 +6311,15 @@
         <v>13</v>
       </c>
       <c r="E82" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="F82" t="s">
-        <v>28</v>
-      </c>
-      <c r="G82" t="s">
-        <v>55</v>
-      </c>
-      <c r="H82" t="s">
-        <v>56</v>
-      </c>
-      <c r="I82" t="s">
-        <v>55</v>
-      </c>
-      <c r="J82" t="s">
-        <v>56</v>
+        <v>124</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="B83" t="s">
         <v>11</v>
@@ -6286,15 +6331,27 @@
         <v>13</v>
       </c>
       <c r="E83" t="s">
-        <v>48</v>
+        <v>96</v>
       </c>
       <c r="F83" t="s">
-        <v>123</v>
+        <v>97</v>
+      </c>
+      <c r="G83" t="s">
+        <v>98</v>
+      </c>
+      <c r="H83" t="s">
+        <v>99</v>
+      </c>
+      <c r="I83" t="s">
+        <v>98</v>
+      </c>
+      <c r="J83" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B84" t="s">
         <v>11</v>
@@ -6306,27 +6363,15 @@
         <v>13</v>
       </c>
       <c r="E84" t="s">
-        <v>96</v>
+        <v>48</v>
       </c>
       <c r="F84" t="s">
-        <v>97</v>
-      </c>
-      <c r="G84" t="s">
-        <v>98</v>
-      </c>
-      <c r="H84" t="s">
-        <v>99</v>
-      </c>
-      <c r="I84" t="s">
-        <v>98</v>
-      </c>
-      <c r="J84" t="s">
-        <v>99</v>
+        <v>160</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B85" t="s">
         <v>11</v>
@@ -6341,49 +6386,61 @@
         <v>48</v>
       </c>
       <c r="F85" t="s">
-        <v>160</v>
+        <v>110</v>
+      </c>
+      <c r="G85" t="s">
+        <v>70</v>
+      </c>
+      <c r="H85" t="s">
+        <v>176</v>
+      </c>
+      <c r="I85" t="s">
+        <v>70</v>
+      </c>
+      <c r="J85" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>197</v>
-      </c>
-      <c r="B86" t="s">
-        <v>11</v>
-      </c>
-      <c r="C86" t="s">
-        <v>12</v>
-      </c>
-      <c r="D86" t="s">
-        <v>13</v>
-      </c>
-      <c r="E86" t="s">
-        <v>48</v>
-      </c>
-      <c r="F86" t="s">
-        <v>141</v>
-      </c>
-      <c r="G86" t="s">
-        <v>70</v>
-      </c>
-      <c r="H86" t="s">
-        <v>176</v>
-      </c>
-      <c r="I86" t="s">
-        <v>70</v>
-      </c>
-      <c r="J86" t="s">
-        <v>176</v>
+        <v>198</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>198</v>
+        <v>199</v>
+      </c>
+      <c r="B87" t="s">
+        <v>11</v>
+      </c>
+      <c r="C87" t="s">
+        <v>12</v>
+      </c>
+      <c r="D87" t="s">
+        <v>13</v>
+      </c>
+      <c r="E87" t="s">
+        <v>27</v>
+      </c>
+      <c r="F87" t="s">
+        <v>28</v>
+      </c>
+      <c r="G87" t="s">
+        <v>29</v>
+      </c>
+      <c r="H87" t="s">
+        <v>30</v>
+      </c>
+      <c r="I87" t="s">
+        <v>29</v>
+      </c>
+      <c r="J87" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B88" t="s">
         <v>11</v>
@@ -6395,27 +6452,27 @@
         <v>13</v>
       </c>
       <c r="E88" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="F88" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="G88" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="H88" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="I88" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="J88" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B89" t="s">
         <v>11</v>
@@ -6427,27 +6484,27 @@
         <v>13</v>
       </c>
       <c r="E89" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="F89" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="G89" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="H89" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="I89" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="J89" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="B90" t="s">
         <v>11</v>
@@ -6459,27 +6516,27 @@
         <v>13</v>
       </c>
       <c r="E90" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="F90" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
       <c r="G90" t="s">
-        <v>16</v>
+        <v>214</v>
       </c>
       <c r="H90" t="s">
-        <v>17</v>
+        <v>215</v>
       </c>
       <c r="I90" t="s">
-        <v>16</v>
+        <v>214</v>
       </c>
       <c r="J90" t="s">
-        <v>17</v>
+        <v>215</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B91" t="s">
         <v>11</v>
@@ -6494,24 +6551,24 @@
         <v>48</v>
       </c>
       <c r="F91" t="s">
-        <v>115</v>
+        <v>49</v>
       </c>
       <c r="G91" t="s">
-        <v>214</v>
+        <v>50</v>
       </c>
       <c r="H91" t="s">
-        <v>215</v>
+        <v>51</v>
       </c>
       <c r="I91" t="s">
-        <v>214</v>
+        <v>50</v>
       </c>
       <c r="J91" t="s">
-        <v>215</v>
+        <v>51</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B92" t="s">
         <v>11</v>
@@ -6523,53 +6580,21 @@
         <v>13</v>
       </c>
       <c r="E92" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="F92" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="G92" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="H92" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="I92" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="J92" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A93" t="s">
-        <v>217</v>
-      </c>
-      <c r="B93" t="s">
-        <v>11</v>
-      </c>
-      <c r="C93" t="s">
-        <v>12</v>
-      </c>
-      <c r="D93" t="s">
-        <v>13</v>
-      </c>
-      <c r="E93" t="s">
-        <v>60</v>
-      </c>
-      <c r="F93" t="s">
-        <v>61</v>
-      </c>
-      <c r="G93" t="s">
-        <v>62</v>
-      </c>
-      <c r="H93" t="s">
-        <v>63</v>
-      </c>
-      <c r="I93" t="s">
-        <v>62</v>
-      </c>
-      <c r="J93" t="s">
         <v>63</v>
       </c>
     </row>
@@ -6579,24 +6604,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF02C4E0-A251-4684-97C1-DCA0C58097F5}">
-  <dimension ref="A1:K28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39D1DDFD-FF0A-4E2A-9CCB-7BEDB7E99244}">
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.86328125" customWidth="1"/>
-    <col min="3" max="3" width="11.3984375" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.73046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.19921875" customWidth="1"/>
+    <col min="3" max="3" width="14.796875" customWidth="1"/>
+    <col min="4" max="4" width="15.86328125" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.06640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.796875" customWidth="1"/>
+    <col min="10" max="10" width="9.86328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
@@ -6667,6 +6693,9 @@
       <c r="A3" t="s">
         <v>58</v>
       </c>
+      <c r="K3" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
@@ -6942,6 +6971,9 @@
       <c r="D13" t="s">
         <v>13</v>
       </c>
+      <c r="K13" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
@@ -7119,7 +7151,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
@@ -7148,7 +7180,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
@@ -7177,7 +7209,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
@@ -7206,7 +7238,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B23" t="s">
         <v>11</v>
@@ -7235,7 +7267,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="B24" t="s">
         <v>11</v>
@@ -7247,21 +7279,24 @@
         <v>13</v>
       </c>
       <c r="E24" t="s">
-        <v>122</v>
+        <v>14</v>
       </c>
       <c r="F24" t="s">
-        <v>141</v>
+        <v>15</v>
       </c>
       <c r="G24" t="s">
-        <v>153</v>
+        <v>16</v>
       </c>
       <c r="H24" t="s">
-        <v>154</v>
+        <v>17</v>
+      </c>
+      <c r="K24" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="B25" t="s">
         <v>11</v>
@@ -7273,21 +7308,18 @@
         <v>13</v>
       </c>
       <c r="E25" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="F25" t="s">
-        <v>15</v>
-      </c>
-      <c r="G25" t="s">
-        <v>16</v>
-      </c>
-      <c r="H25" t="s">
-        <v>17</v>
+        <v>124</v>
+      </c>
+      <c r="K25" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="B26" t="s">
         <v>11</v>
@@ -7302,32 +7334,18 @@
         <v>48</v>
       </c>
       <c r="F26" t="s">
-        <v>123</v>
+        <v>160</v>
+      </c>
+      <c r="K26" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>196</v>
-      </c>
-      <c r="B27" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" t="s">
-        <v>48</v>
-      </c>
-      <c r="F27" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
         <v>198</v>
+      </c>
+      <c r="K27" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>